<commit_message>
Rai dai ko struc dwg complete and kurthali truss estimate completed
</commit_message>
<xml_diff>
--- a/ofc/estimates/kurthali truss/truss.xlsx
+++ b/ofc/estimates/kurthali truss/truss.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="18" r:id="rId1"/>
+    <sheet name="as per mistry" sheetId="19" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="adopted_rate_aggregate_10_20_mm">[1]District_Rate!$L$6</definedName>
@@ -40,7 +41,9 @@
     <definedName name="description_784">[2]Abstract!$B$300</definedName>
     <definedName name="excavator">[1]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[1]Equipment_Rate!$J$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'as per mistry'!$A$1:$K$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$62</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'as per mistry'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">new!$1:$8</definedName>
     <definedName name="skilled">[1]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[1]District_Rate!$D$149</definedName>
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -212,6 +215,36 @@
   </si>
   <si>
     <t xml:space="preserve">d]lzgsf] k|of]u u/L ;'k/ :6«Sr/df l;d]G6 s+lqm6 ug]{ sfd -!M!=%M#_ </t>
+  </si>
+  <si>
+    <t>-MS square pipe of 3" * 3" of 1.8mm thickness for vertical post</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 2"*2" of 1.8mm thickness for horizontal member</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 2"*2" of 1.6mm thickness for king post member</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 1.5"*1.5" of 1.6mm thickness for vertical member</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 1.5"*1.5" of 1.6mm thickness for diagnol member</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 2"*2" of 1.8mm thickness for inclined member</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 2"*2" of 1.8mm thickness for purlins</t>
+  </si>
+  <si>
+    <t>e'O{+tNnfdf lrDgL e§fsf] O{+6fsf] uf/f] l;d]G6 d;nf -!M^_ df</t>
+  </si>
+  <si>
+    <t>;'Vvf O{6f RofK6f] 5fKg] sfd</t>
+  </si>
+  <si>
+    <t>no.</t>
   </si>
 </sst>
 </file>
@@ -491,26 +524,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,8 +543,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1196,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
@@ -1220,113 +1253,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="44" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -2324,7 +2357,7 @@
       <c r="A51" s="21">
         <v>3</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="41" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="22">
@@ -2366,7 +2399,7 @@
       <c r="A53" s="21">
         <v>4</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C53" s="22">
@@ -2449,11 +2482,11 @@
       <c r="B57" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C57" s="48">
         <f>J55</f>
         <v>618050.76766828669</v>
       </c>
-      <c r="D57" s="42"/>
+      <c r="D57" s="49"/>
       <c r="E57" s="10">
         <v>100</v>
       </c>
@@ -2487,10 +2520,10 @@
       <c r="B58" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="45">
+      <c r="C58" s="51">
         <v>400000</v>
       </c>
-      <c r="D58" s="46"/>
+      <c r="D58" s="52"/>
       <c r="E58" s="10"/>
       <c r="M58" s="29"/>
       <c r="N58" s="30"/>
@@ -2516,11 +2549,11 @@
       <c r="B59" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="45">
+      <c r="C59" s="51">
         <f>C58-C61-C62</f>
         <v>380000</v>
       </c>
-      <c r="D59" s="46"/>
+      <c r="D59" s="52"/>
       <c r="E59" s="10">
         <f>C59/C57*100</f>
         <v>61.483622362224679</v>
@@ -2549,11 +2582,11 @@
       <c r="B60" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="47">
+      <c r="C60" s="53">
         <f>C57-C59</f>
         <v>238050.76766828669</v>
       </c>
-      <c r="D60" s="47"/>
+      <c r="D60" s="53"/>
       <c r="E60" s="10">
         <f>100-E59</f>
         <v>38.516377637775321</v>
@@ -2582,11 +2615,11 @@
       <c r="B61" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="48">
         <f>C58*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D61" s="42"/>
+      <c r="D61" s="49"/>
       <c r="E61" s="10">
         <v>3</v>
       </c>
@@ -2614,11 +2647,11 @@
       <c r="B62" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="41">
+      <c r="C62" s="48">
         <f>C58*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D62" s="42"/>
+      <c r="D62" s="49"/>
       <c r="E62" s="10">
         <v>2</v>
       </c>
@@ -2644,13 +2677,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="A7:F7"/>
@@ -2659,6 +2685,1632 @@
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+    </row>
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>1</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="40">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D10" s="10">
+        <f>(2.5+1.5+13)/3.281</f>
+        <v>5.1813471502590671</v>
+      </c>
+      <c r="E10" s="10">
+        <v>3.97</v>
+      </c>
+      <c r="F10" s="10">
+        <f>PRODUCT(C10:E10)</f>
+        <v>308.54922279792743</v>
+      </c>
+      <c r="G10" s="36">
+        <f>F10</f>
+        <v>308.54922279792743</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="11"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="40">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10">
+        <f>(1.5+30+1.5)/3.281</f>
+        <v>10.057909174032307</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2.72</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" ref="F11:F21" si="0">PRODUCT(C11:E11)</f>
+        <v>136.78756476683938</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" ref="G11:G21" si="1">F11</f>
+        <v>136.78756476683938</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="11"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="40">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D12" s="10">
+        <f>16.333/3.281</f>
+        <v>4.97805547089302</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2.72</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>135.40310880829014</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="1"/>
+        <v>135.40310880829014</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="11"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="40">
+        <f>1*5</f>
+        <v>5</v>
+      </c>
+      <c r="D13" s="10">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="E13" s="10">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>12.960987503809815</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="1"/>
+        <v>12.960987503809815</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="40">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D14" s="10">
+        <f>4/3.281</f>
+        <v>1.2191405059433098</v>
+      </c>
+      <c r="E14" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>47.180737580006088</v>
+      </c>
+      <c r="G14" s="36">
+        <f t="shared" si="1"/>
+        <v>47.180737580006088</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="11"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40">
+        <f t="shared" ref="C15:C21" si="2">2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D15" s="10">
+        <f>3.583/3.281</f>
+        <v>1.0920451081987199</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>42.262145687290463</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" si="1"/>
+        <v>42.262145687290463</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="11"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="10">
+        <f>3.25/3.281</f>
+        <v>0.99055166107893933</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>38.334349283754953</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="1"/>
+        <v>38.334349283754953</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="11"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D17" s="10">
+        <f>3.083/3.281</f>
+        <v>0.93965254495580619</v>
+      </c>
+      <c r="E17" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>36.364553489789699</v>
+      </c>
+      <c r="G17" s="36">
+        <f t="shared" si="1"/>
+        <v>36.364553489789699</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="11"/>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="10">
+        <f>2.667/3.281</f>
+        <v>0.81286193233770188</v>
+      </c>
+      <c r="E18" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="0"/>
+        <v>31.457756781469062</v>
+      </c>
+      <c r="G18" s="36">
+        <f t="shared" si="1"/>
+        <v>31.457756781469062</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="11"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D19" s="10">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E19" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="0"/>
+        <v>23.590368790003044</v>
+      </c>
+      <c r="G19" s="36">
+        <f t="shared" si="1"/>
+        <v>23.590368790003044</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="11"/>
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D20" s="10">
+        <f>1.333/3.281</f>
+        <v>0.40627857360560804</v>
+      </c>
+      <c r="E20" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="0"/>
+        <v>15.72298079853703</v>
+      </c>
+      <c r="G20" s="36">
+        <f t="shared" si="1"/>
+        <v>15.72298079853703</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="11"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D21" s="10">
+        <f>8/12/3.281</f>
+        <v>0.20319008432388497</v>
+      </c>
+      <c r="E21" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="0"/>
+        <v>7.8634562633343483</v>
+      </c>
+      <c r="G21" s="36">
+        <f t="shared" si="1"/>
+        <v>7.8634562633343483</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="11"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="38"/>
+      <c r="B22" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="40">
+        <f>2*6</f>
+        <v>12</v>
+      </c>
+      <c r="D22" s="10">
+        <f>44/3.281</f>
+        <v>13.41054556537641</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2.72</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" ref="F22" si="3">PRODUCT(C22:E22)</f>
+        <v>437.72020725388603</v>
+      </c>
+      <c r="G22" s="36">
+        <f t="shared" ref="G22" si="4">F22</f>
+        <v>437.72020725388603</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="11"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="27">
+        <f>SUM(G10:G22)</f>
+        <v>1274.1974398049376</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="26">
+        <v>181.17</v>
+      </c>
+      <c r="J23" s="27">
+        <f>G23*I23</f>
+        <v>230846.35016946052</v>
+      </c>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27">
+        <f>0.13*G23*(1871.42/18.94)</f>
+        <v>16367.086296936026</v>
+      </c>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+      <c r="A26" s="38">
+        <v>2</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="11"/>
+      <c r="M26" s="12"/>
+    </row>
+    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40">
+        <v>2</v>
+      </c>
+      <c r="D27" s="10">
+        <f>16.333/3.281</f>
+        <v>4.97805547089302</v>
+      </c>
+      <c r="E27" s="10">
+        <f>44/3.281</f>
+        <v>13.41054556537641</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="36">
+        <f>PRODUCT(C27:F27)</f>
+        <v>133.51687943876433</v>
+      </c>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="11"/>
+      <c r="M27" s="12"/>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="27">
+        <f>SUM(G27:G27)</f>
+        <v>133.51687943876433</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="26">
+        <v>1070.9000000000001</v>
+      </c>
+      <c r="J28" s="27">
+        <f>G28*I28</f>
+        <v>142983.22619097272</v>
+      </c>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27">
+        <f>0.13*G28*8587.63/10</f>
+        <v>14905.716271871303</v>
+      </c>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A31" s="21">
+        <v>3</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="22">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D32" s="23">
+        <v>0.45</v>
+      </c>
+      <c r="E32" s="24">
+        <v>0.45</v>
+      </c>
+      <c r="F32" s="24">
+        <f>(2.5+0.25+0.17)/3.281</f>
+        <v>0.88997256933861624</v>
+      </c>
+      <c r="G32" s="36">
+        <f>PRODUCT(C32:F32)</f>
+        <v>2.7032916793660471</v>
+      </c>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="27">
+        <f>SUM(G32:G32)</f>
+        <v>2.7032916793660471</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J33" s="27">
+        <f>G33*I33</f>
+        <v>1793.1204038402925</v>
+      </c>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="21">
+        <v>4</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="22">
+        <f>C32</f>
+        <v>15</v>
+      </c>
+      <c r="D36" s="23">
+        <f>D32</f>
+        <v>0.45</v>
+      </c>
+      <c r="E36" s="24">
+        <f>E32</f>
+        <v>0.45</v>
+      </c>
+      <c r="F36" s="24"/>
+      <c r="G36" s="36">
+        <f>PRODUCT(C36:F36)</f>
+        <v>3.0375000000000001</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="27">
+        <f>SUM(G36:G36)</f>
+        <v>3.0375000000000001</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="26">
+        <v>1014.97</v>
+      </c>
+      <c r="J37" s="27">
+        <f>G37*I37</f>
+        <v>3082.9713750000001</v>
+      </c>
+      <c r="K37" s="24"/>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27">
+        <f>0.13*G37*8617.2/10</f>
+        <v>340.27168500000005</v>
+      </c>
+      <c r="K38" s="24"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A40" s="21">
+        <v>5</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="24"/>
+    </row>
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="21"/>
+      <c r="B41" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="22">
+        <f>C36</f>
+        <v>15</v>
+      </c>
+      <c r="D41" s="23">
+        <f>D36</f>
+        <v>0.45</v>
+      </c>
+      <c r="E41" s="24">
+        <f>E36</f>
+        <v>0.45</v>
+      </c>
+      <c r="F41" s="24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G41" s="36">
+        <f>PRODUCT(C41:F41)</f>
+        <v>0.2278125</v>
+      </c>
+      <c r="H41" s="25"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="21"/>
+      <c r="B42" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="27">
+        <f>SUM(G41:G41)</f>
+        <v>0.2278125</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J42" s="27">
+        <f>G42*I42</f>
+        <v>2957.71246875</v>
+      </c>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="B43" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="27">
+        <f>0.13*G42*8078.11</f>
+        <v>239.23827646874997</v>
+      </c>
+      <c r="K43" s="24"/>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="24"/>
+    </row>
+    <row r="45" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A45" s="21">
+        <v>6</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="22">
+        <f>C41</f>
+        <v>15</v>
+      </c>
+      <c r="D46" s="23">
+        <f>D41</f>
+        <v>0.45</v>
+      </c>
+      <c r="E46" s="24">
+        <f>E41</f>
+        <v>0.45</v>
+      </c>
+      <c r="F46" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="G46" s="36">
+        <f>PRODUCT(C46:F46)</f>
+        <v>2.2781250000000002</v>
+      </c>
+      <c r="H46" s="25"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="22">
+        <f>C46</f>
+        <v>15</v>
+      </c>
+      <c r="D47" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E47" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F47" s="24">
+        <v>0.45</v>
+      </c>
+      <c r="G47" s="36">
+        <f>PRODUCT(C47:F47)</f>
+        <v>0.60749999999999993</v>
+      </c>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="21"/>
+      <c r="B48" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="27">
+        <f>SUM(G46:G47)</f>
+        <v>2.8856250000000001</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I48" s="26">
+        <v>13568.9</v>
+      </c>
+      <c r="J48" s="27">
+        <f>G48*I48</f>
+        <v>39154.757062500001</v>
+      </c>
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27">
+        <f>0.13*G48*9524.2</f>
+        <v>3572.8250512500003</v>
+      </c>
+      <c r="K49" s="24"/>
+    </row>
+    <row r="50" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="21"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="24"/>
+    </row>
+    <row r="51" spans="1:31" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A51" s="21">
+        <v>7</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="21"/>
+      <c r="B52" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="22">
+        <f>4*2</f>
+        <v>8</v>
+      </c>
+      <c r="D52" s="23">
+        <f>13.917/3.281</f>
+        <v>4.2416946053032607</v>
+      </c>
+      <c r="E52" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F52" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G52" s="36">
+        <f>PRODUCT(C52:F52)</f>
+        <v>2.3414154221273997</v>
+      </c>
+      <c r="H52" s="25"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="22">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="D53" s="23">
+        <f>8.917/3.281</f>
+        <v>2.7177689728741234</v>
+      </c>
+      <c r="E53" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F53" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G53" s="36">
+        <f>PRODUCT(C53:F53)</f>
+        <v>0.75010423651325808</v>
+      </c>
+      <c r="H53" s="25"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="24"/>
+    </row>
+    <row r="54" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="27">
+        <f>SUM(G52:G53)</f>
+        <v>3.0915196586406579</v>
+      </c>
+      <c r="H54" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I54" s="26">
+        <v>14362.76</v>
+      </c>
+      <c r="J54" s="27">
+        <f>G54*I54</f>
+        <v>44402.754892337696</v>
+      </c>
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27">
+        <f>0.13*G54*10311.74</f>
+        <v>4144.2631002228582</v>
+      </c>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="21"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="24"/>
+    </row>
+    <row r="57" spans="1:31" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="21">
+        <v>8</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="22">
+        <v>1</v>
+      </c>
+      <c r="D57" s="23"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="36">
+        <f>PRODUCT(C57:F57)</f>
+        <v>1</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I57" s="26">
+        <v>5000</v>
+      </c>
+      <c r="J57" s="27">
+        <f>G57*I57</f>
+        <v>5000</v>
+      </c>
+      <c r="K57" s="24"/>
+    </row>
+    <row r="58" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="24"/>
+    </row>
+    <row r="59" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21">
+        <v>9</v>
+      </c>
+      <c r="B59" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="22">
+        <v>1</v>
+      </c>
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="36">
+        <f>PRODUCT(C59:F59)</f>
+        <v>1</v>
+      </c>
+      <c r="H59" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" s="26">
+        <v>500</v>
+      </c>
+      <c r="J59" s="27">
+        <f>G59*I59</f>
+        <v>500</v>
+      </c>
+      <c r="K59" s="24"/>
+    </row>
+    <row r="60" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="21"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="24"/>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
+      <c r="B61" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7">
+        <f>SUM(J10:J60)</f>
+        <v>510290.29324461019</v>
+      </c>
+      <c r="K61" s="4"/>
+      <c r="M61" s="29"/>
+      <c r="P61" s="32"/>
+      <c r="Q61" s="32"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="M62" s="29"/>
+      <c r="N62" s="30"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="31"/>
+      <c r="R62" s="30"/>
+      <c r="S62" s="30"/>
+      <c r="T62" s="30"/>
+      <c r="U62" s="29"/>
+      <c r="V62" s="29"/>
+      <c r="W62" s="29"/>
+      <c r="X62" s="29"/>
+      <c r="Y62" s="29"/>
+      <c r="Z62" s="29"/>
+      <c r="AA62" s="29"/>
+      <c r="AB62" s="29"/>
+      <c r="AC62" s="29"/>
+      <c r="AD62" s="29"/>
+      <c r="AE62" s="29"/>
+    </row>
+    <row r="63" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="48">
+        <f>J61</f>
+        <v>510290.29324461019</v>
+      </c>
+      <c r="D63" s="49"/>
+      <c r="E63" s="10">
+        <v>100</v>
+      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="16"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="30"/>
+      <c r="O63" s="30"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="30"/>
+      <c r="R63" s="30"/>
+      <c r="S63" s="30"/>
+      <c r="T63" s="30"/>
+      <c r="U63" s="12"/>
+      <c r="V63" s="12"/>
+      <c r="W63" s="12"/>
+      <c r="X63" s="12"/>
+      <c r="Y63" s="12"/>
+      <c r="Z63" s="12"/>
+      <c r="AA63" s="12"/>
+      <c r="AB63" s="12"/>
+      <c r="AC63" s="12"/>
+      <c r="AD63" s="12"/>
+      <c r="AE63" s="12"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B64" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="51">
+        <v>400000</v>
+      </c>
+      <c r="D64" s="52"/>
+      <c r="E64" s="10"/>
+      <c r="M64" s="29"/>
+      <c r="N64" s="30"/>
+      <c r="O64" s="30"/>
+      <c r="P64" s="30"/>
+      <c r="Q64" s="30"/>
+      <c r="R64" s="30"/>
+      <c r="S64" s="30"/>
+      <c r="T64" s="30"/>
+      <c r="U64" s="29"/>
+      <c r="V64" s="29"/>
+      <c r="W64" s="29"/>
+      <c r="X64" s="29"/>
+      <c r="Y64" s="29"/>
+      <c r="Z64" s="29"/>
+      <c r="AA64" s="29"/>
+      <c r="AB64" s="29"/>
+      <c r="AC64" s="29"/>
+      <c r="AD64" s="29"/>
+      <c r="AE64" s="29"/>
+    </row>
+    <row r="65" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B65" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="51">
+        <f>C64-C67-C68</f>
+        <v>380000</v>
+      </c>
+      <c r="D65" s="52"/>
+      <c r="E65" s="10">
+        <f>C65/C63*100</f>
+        <v>74.467416886145841</v>
+      </c>
+      <c r="M65" s="29"/>
+      <c r="N65" s="29"/>
+      <c r="O65" s="29"/>
+      <c r="P65" s="29"/>
+      <c r="Q65" s="29"/>
+      <c r="R65" s="29"/>
+      <c r="S65" s="29"/>
+      <c r="T65" s="29"/>
+      <c r="U65" s="29"/>
+      <c r="V65" s="29"/>
+      <c r="W65" s="29"/>
+      <c r="X65" s="29"/>
+      <c r="Y65" s="29"/>
+      <c r="Z65" s="29"/>
+      <c r="AA65" s="29"/>
+      <c r="AB65" s="29"/>
+      <c r="AC65" s="29"/>
+      <c r="AD65" s="29"/>
+      <c r="AE65" s="29"/>
+    </row>
+    <row r="66" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B66" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="53">
+        <f>C63-C65</f>
+        <v>130290.29324461019</v>
+      </c>
+      <c r="D66" s="53"/>
+      <c r="E66" s="10">
+        <f>100-E65</f>
+        <v>25.532583113854159</v>
+      </c>
+      <c r="M66" s="29"/>
+      <c r="N66" s="29"/>
+      <c r="O66" s="29"/>
+      <c r="P66" s="29"/>
+      <c r="Q66" s="29"/>
+      <c r="R66" s="29"/>
+      <c r="S66" s="29"/>
+      <c r="T66" s="29"/>
+      <c r="U66" s="29"/>
+      <c r="V66" s="29"/>
+      <c r="W66" s="29"/>
+      <c r="X66" s="29"/>
+      <c r="Y66" s="29"/>
+      <c r="Z66" s="29"/>
+      <c r="AA66" s="29"/>
+      <c r="AB66" s="29"/>
+      <c r="AC66" s="29"/>
+      <c r="AD66" s="29"/>
+      <c r="AE66" s="29"/>
+    </row>
+    <row r="67" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B67" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="48">
+        <f>C64*0.03</f>
+        <v>12000</v>
+      </c>
+      <c r="D67" s="49"/>
+      <c r="E67" s="10">
+        <v>3</v>
+      </c>
+      <c r="M67" s="29"/>
+      <c r="N67" s="29"/>
+      <c r="O67" s="29"/>
+      <c r="P67" s="29"/>
+      <c r="Q67" s="29"/>
+      <c r="R67" s="29"/>
+      <c r="S67" s="29"/>
+      <c r="T67" s="29"/>
+      <c r="U67" s="29"/>
+      <c r="V67" s="29"/>
+      <c r="W67" s="29"/>
+      <c r="X67" s="29"/>
+      <c r="Y67" s="29"/>
+      <c r="Z67" s="29"/>
+      <c r="AA67" s="29"/>
+      <c r="AB67" s="29"/>
+      <c r="AC67" s="29"/>
+      <c r="AD67" s="29"/>
+      <c r="AE67" s="29"/>
+    </row>
+    <row r="68" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B68" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="48">
+        <f>C64*0.02</f>
+        <v>8000</v>
+      </c>
+      <c r="D68" s="49"/>
+      <c r="E68" s="10">
+        <v>2</v>
+      </c>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
+      <c r="O68" s="29"/>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29"/>
+      <c r="S68" s="29"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="29"/>
+      <c r="V68" s="29"/>
+      <c r="W68" s="29"/>
+      <c r="X68" s="29"/>
+      <c r="Y68" s="29"/>
+      <c r="Z68" s="29"/>
+      <c r="AA68" s="29"/>
+      <c r="AB68" s="29"/>
+      <c r="AC68" s="29"/>
+      <c r="AD68" s="29"/>
+      <c r="AE68" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>